<commit_message>
removed panda and numpy
</commit_message>
<xml_diff>
--- a/tests/test1/BOM_1.1.xlsx
+++ b/tests/test1/BOM_1.1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ASETS-code\python\pyp-id_finder\tests\test1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA96CECC-BD73-45F6-A534-C730161640F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECC3B2E7-A9F5-4415-9723-680A3E27A696}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="132">
   <si>
     <t>#</t>
   </si>
@@ -391,6 +391,9 @@
   </si>
   <si>
     <t>G920</t>
+  </si>
+  <si>
+    <t>Pompa 1</t>
   </si>
   <si>
     <t>Pompa chiller</t>
@@ -442,11 +445,18 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -583,46 +593,43 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -633,54 +640,61 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -899,13 +913,13 @@
   <sheetPr>
     <tabColor rgb="FFFFFF99"/>
   </sheetPr>
-  <dimension ref="A1:AH46"/>
+  <dimension ref="A1:AH47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F29" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="F32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A38" sqref="A38:XFD38"/>
+      <selection pane="bottomRight" activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2698,11 +2712,11 @@
       <c r="J37" s="8"/>
       <c r="K37" s="8"/>
       <c r="L37" s="8"/>
-      <c r="M37" s="9" t="s">
-        <v>43</v>
+      <c r="M37" s="18" t="s">
+        <v>117</v>
       </c>
       <c r="N37" s="9" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="O37" s="8"/>
       <c r="P37" s="9"/>
@@ -2725,131 +2739,136 @@
       <c r="AG37" s="8"/>
       <c r="AH37" s="13"/>
     </row>
-    <row r="38" spans="1:34" s="24" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="18"/>
-      <c r="B38" s="18"/>
-      <c r="C38" s="18"/>
-      <c r="D38" s="18"/>
-      <c r="E38" s="19"/>
-      <c r="F38" s="18"/>
-      <c r="G38" s="18"/>
-      <c r="H38" s="18"/>
-      <c r="I38" s="18"/>
-      <c r="J38" s="18"/>
-      <c r="K38" s="18"/>
-      <c r="L38" s="18"/>
-      <c r="M38" s="20"/>
-      <c r="N38" s="20"/>
-      <c r="O38" s="18"/>
-      <c r="P38" s="20"/>
-      <c r="Q38" s="21"/>
-      <c r="R38" s="18"/>
-      <c r="S38" s="18"/>
-      <c r="T38" s="18"/>
-      <c r="U38" s="18"/>
-      <c r="V38" s="18"/>
-      <c r="W38" s="18"/>
-      <c r="X38" s="20"/>
-      <c r="Y38" s="20"/>
-      <c r="Z38" s="22"/>
-      <c r="AA38" s="20"/>
-      <c r="AB38" s="18"/>
-      <c r="AC38" s="18"/>
-      <c r="AD38" s="20"/>
-      <c r="AE38" s="20"/>
-      <c r="AF38" s="20"/>
-      <c r="AG38" s="18"/>
-      <c r="AH38" s="23"/>
-    </row>
-    <row r="39" spans="1:34" s="34" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="25">
+    <row r="38" spans="1:34" s="25" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="19"/>
+      <c r="B38" s="19"/>
+      <c r="C38" s="19"/>
+      <c r="D38" s="19"/>
+      <c r="E38" s="20"/>
+      <c r="F38" s="19"/>
+      <c r="G38" s="19"/>
+      <c r="H38" s="19"/>
+      <c r="I38" s="19"/>
+      <c r="J38" s="19"/>
+      <c r="K38" s="19"/>
+      <c r="L38" s="19"/>
+      <c r="M38" s="21"/>
+      <c r="N38" s="21"/>
+      <c r="O38" s="19"/>
+      <c r="P38" s="21"/>
+      <c r="Q38" s="22"/>
+      <c r="R38" s="19"/>
+      <c r="S38" s="19"/>
+      <c r="T38" s="19"/>
+      <c r="U38" s="19"/>
+      <c r="V38" s="19"/>
+      <c r="W38" s="19"/>
+      <c r="X38" s="21"/>
+      <c r="Y38" s="21"/>
+      <c r="Z38" s="23"/>
+      <c r="AA38" s="21"/>
+      <c r="AB38" s="19"/>
+      <c r="AC38" s="19"/>
+      <c r="AD38" s="21"/>
+      <c r="AE38" s="21"/>
+      <c r="AF38" s="21"/>
+      <c r="AG38" s="19"/>
+      <c r="AH38" s="24"/>
+    </row>
+    <row r="39" spans="1:34" s="35" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="26">
         <v>282</v>
       </c>
-      <c r="B39" s="26" t="s">
-        <v>118</v>
-      </c>
-      <c r="C39" s="25">
+      <c r="B39" s="27" t="s">
+        <v>119</v>
+      </c>
+      <c r="C39" s="26">
         <v>141</v>
       </c>
-      <c r="D39" s="27"/>
-      <c r="E39" s="25" t="s">
-        <v>119</v>
-      </c>
-      <c r="F39" s="25" t="s">
+      <c r="D39" s="28"/>
+      <c r="E39" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="G39" s="25" t="s">
+      <c r="F39" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="G39" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="H39" s="28"/>
-      <c r="I39" s="28"/>
-      <c r="J39" s="28"/>
-      <c r="K39" s="28"/>
-      <c r="L39" s="25" t="s">
-        <v>121</v>
-      </c>
-      <c r="M39" s="29" t="s">
+      <c r="H39" s="29"/>
+      <c r="I39" s="29"/>
+      <c r="J39" s="29"/>
+      <c r="K39" s="29"/>
+      <c r="L39" s="26" t="s">
         <v>122</v>
       </c>
-      <c r="N39" s="30" t="s">
+      <c r="M39" s="30" t="s">
         <v>123</v>
       </c>
-      <c r="O39" s="25" t="s">
+      <c r="N39" s="31" t="s">
         <v>124</v>
       </c>
-      <c r="P39" s="29" t="s">
+      <c r="O39" s="26" t="s">
         <v>125</v>
       </c>
-      <c r="Q39" s="31" t="s">
+      <c r="P39" s="30" t="s">
         <v>126</v>
       </c>
-      <c r="R39" s="25">
+      <c r="Q39" s="32" t="s">
+        <v>127</v>
+      </c>
+      <c r="R39" s="26">
         <v>3</v>
       </c>
-      <c r="S39" s="25"/>
-      <c r="T39" s="25"/>
-      <c r="U39" s="25" t="s">
+      <c r="S39" s="26"/>
+      <c r="T39" s="26"/>
+      <c r="U39" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="V39" s="33" t="s">
         <v>127</v>
       </c>
-      <c r="V39" s="32" t="s">
-        <v>126</v>
-      </c>
-      <c r="W39" s="25" t="s">
-        <v>126</v>
-      </c>
-      <c r="X39" s="29" t="s">
-        <v>128</v>
-      </c>
-      <c r="Y39" s="29"/>
-      <c r="Z39" s="27"/>
-      <c r="AA39" s="29" t="s">
+      <c r="W39" s="26" t="s">
+        <v>127</v>
+      </c>
+      <c r="X39" s="30" t="s">
         <v>129</v>
       </c>
-      <c r="AB39" s="25" t="s">
+      <c r="Y39" s="30"/>
+      <c r="Z39" s="28"/>
+      <c r="AA39" s="30" t="s">
         <v>130</v>
       </c>
-      <c r="AC39" s="25"/>
-      <c r="AD39" s="29"/>
-      <c r="AE39" s="29"/>
-      <c r="AF39" s="29"/>
-      <c r="AG39" s="25"/>
-      <c r="AH39" s="33"/>
+      <c r="AB39" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="AC39" s="26"/>
+      <c r="AD39" s="30"/>
+      <c r="AE39" s="30"/>
+      <c r="AF39" s="30"/>
+      <c r="AG39" s="26"/>
+      <c r="AH39" s="34"/>
+    </row>
+    <row r="40" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E40" s="17"/>
     </row>
     <row r="41" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F41" s="17"/>
     </row>
     <row r="42" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F42" s="17"/>
+      <c r="F42" s="36"/>
     </row>
     <row r="44" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G44" s="17"/>
     </row>
     <row r="45" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E45" s="17"/>
+      <c r="H45" s="17"/>
     </row>
     <row r="46" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G46" s="17"/>
     </row>
+    <row r="47" spans="1:34" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <autoFilter ref="A1:AJ39" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>

<commit_message>
created sorting excell by P&ID tag
</commit_message>
<xml_diff>
--- a/tests/test1/BOM_1.1.xlsx
+++ b/tests/test1/BOM_1.1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ASETS-code\python\pyp-id_finder\tests\test1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECC3B2E7-A9F5-4415-9723-680A3E27A696}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{340F68B4-1163-475D-9874-0EEF3664752A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -647,6 +647,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -694,7 +695,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -919,7 +919,7 @@
       <pane xSplit="5" ySplit="1" topLeftCell="F32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="F42" sqref="F42"/>
+      <selection pane="bottomRight" activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2739,115 +2739,115 @@
       <c r="AG37" s="8"/>
       <c r="AH37" s="13"/>
     </row>
-    <row r="38" spans="1:34" s="25" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="19"/>
-      <c r="B38" s="19"/>
-      <c r="C38" s="19"/>
-      <c r="D38" s="19"/>
-      <c r="E38" s="20"/>
-      <c r="F38" s="19"/>
-      <c r="G38" s="19"/>
-      <c r="H38" s="19"/>
-      <c r="I38" s="19"/>
-      <c r="J38" s="19"/>
-      <c r="K38" s="19"/>
-      <c r="L38" s="19"/>
-      <c r="M38" s="21"/>
-      <c r="N38" s="21"/>
-      <c r="O38" s="19"/>
-      <c r="P38" s="21"/>
-      <c r="Q38" s="22"/>
-      <c r="R38" s="19"/>
-      <c r="S38" s="19"/>
-      <c r="T38" s="19"/>
-      <c r="U38" s="19"/>
-      <c r="V38" s="19"/>
-      <c r="W38" s="19"/>
-      <c r="X38" s="21"/>
-      <c r="Y38" s="21"/>
-      <c r="Z38" s="23"/>
-      <c r="AA38" s="21"/>
-      <c r="AB38" s="19"/>
-      <c r="AC38" s="19"/>
-      <c r="AD38" s="21"/>
-      <c r="AE38" s="21"/>
-      <c r="AF38" s="21"/>
-      <c r="AG38" s="19"/>
-      <c r="AH38" s="24"/>
-    </row>
-    <row r="39" spans="1:34" s="35" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="26">
+    <row r="38" spans="1:34" s="26" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="20"/>
+      <c r="B38" s="20"/>
+      <c r="C38" s="20"/>
+      <c r="D38" s="20"/>
+      <c r="E38" s="21"/>
+      <c r="F38" s="20"/>
+      <c r="G38" s="20"/>
+      <c r="H38" s="20"/>
+      <c r="I38" s="20"/>
+      <c r="J38" s="20"/>
+      <c r="K38" s="20"/>
+      <c r="L38" s="20"/>
+      <c r="M38" s="22"/>
+      <c r="N38" s="22"/>
+      <c r="O38" s="20"/>
+      <c r="P38" s="22"/>
+      <c r="Q38" s="23"/>
+      <c r="R38" s="20"/>
+      <c r="S38" s="20"/>
+      <c r="T38" s="20"/>
+      <c r="U38" s="20"/>
+      <c r="V38" s="20"/>
+      <c r="W38" s="20"/>
+      <c r="X38" s="22"/>
+      <c r="Y38" s="22"/>
+      <c r="Z38" s="24"/>
+      <c r="AA38" s="22"/>
+      <c r="AB38" s="20"/>
+      <c r="AC38" s="20"/>
+      <c r="AD38" s="22"/>
+      <c r="AE38" s="22"/>
+      <c r="AF38" s="22"/>
+      <c r="AG38" s="20"/>
+      <c r="AH38" s="25"/>
+    </row>
+    <row r="39" spans="1:34" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="27">
         <v>282</v>
       </c>
-      <c r="B39" s="27" t="s">
+      <c r="B39" s="28" t="s">
         <v>119</v>
       </c>
-      <c r="C39" s="26">
+      <c r="C39" s="27">
         <v>141</v>
       </c>
-      <c r="D39" s="28"/>
-      <c r="E39" s="26" t="s">
+      <c r="D39" s="29"/>
+      <c r="E39" s="27" t="s">
         <v>120</v>
       </c>
-      <c r="F39" s="26" t="s">
+      <c r="F39" s="27" t="s">
         <v>121</v>
       </c>
-      <c r="G39" s="26" t="s">
+      <c r="G39" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="H39" s="29"/>
-      <c r="I39" s="29"/>
-      <c r="J39" s="29"/>
-      <c r="K39" s="29"/>
-      <c r="L39" s="26" t="s">
+      <c r="H39" s="30"/>
+      <c r="I39" s="30"/>
+      <c r="J39" s="30"/>
+      <c r="K39" s="30"/>
+      <c r="L39" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="M39" s="30" t="s">
+      <c r="M39" s="31" t="s">
         <v>123</v>
       </c>
-      <c r="N39" s="31" t="s">
+      <c r="N39" s="32" t="s">
         <v>124</v>
       </c>
-      <c r="O39" s="26" t="s">
+      <c r="O39" s="27" t="s">
         <v>125</v>
       </c>
-      <c r="P39" s="30" t="s">
+      <c r="P39" s="31" t="s">
         <v>126</v>
       </c>
-      <c r="Q39" s="32" t="s">
+      <c r="Q39" s="33" t="s">
         <v>127</v>
       </c>
-      <c r="R39" s="26">
+      <c r="R39" s="27">
         <v>3</v>
       </c>
-      <c r="S39" s="26"/>
-      <c r="T39" s="26"/>
-      <c r="U39" s="26" t="s">
+      <c r="S39" s="27"/>
+      <c r="T39" s="27"/>
+      <c r="U39" s="27" t="s">
         <v>128</v>
       </c>
-      <c r="V39" s="33" t="s">
+      <c r="V39" s="34" t="s">
         <v>127</v>
       </c>
-      <c r="W39" s="26" t="s">
+      <c r="W39" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="X39" s="30" t="s">
+      <c r="X39" s="31" t="s">
         <v>129</v>
       </c>
-      <c r="Y39" s="30"/>
-      <c r="Z39" s="28"/>
-      <c r="AA39" s="30" t="s">
+      <c r="Y39" s="31"/>
+      <c r="Z39" s="29"/>
+      <c r="AA39" s="31" t="s">
         <v>130</v>
       </c>
-      <c r="AB39" s="26" t="s">
+      <c r="AB39" s="27" t="s">
         <v>131</v>
       </c>
-      <c r="AC39" s="26"/>
-      <c r="AD39" s="30"/>
-      <c r="AE39" s="30"/>
-      <c r="AF39" s="30"/>
-      <c r="AG39" s="26"/>
-      <c r="AH39" s="34"/>
+      <c r="AC39" s="27"/>
+      <c r="AD39" s="31"/>
+      <c r="AE39" s="31"/>
+      <c r="AF39" s="31"/>
+      <c r="AG39" s="27"/>
+      <c r="AH39" s="35"/>
     </row>
     <row r="40" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E40" s="17"/>
@@ -2856,7 +2856,10 @@
       <c r="F41" s="17"/>
     </row>
     <row r="42" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F42" s="36"/>
+      <c r="F42" s="19"/>
+    </row>
+    <row r="43" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F43" s="17"/>
     </row>
     <row r="44" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G44" s="17"/>

</xml_diff>